<commit_message>
Uploading changes from the last test
</commit_message>
<xml_diff>
--- a/score_data.xlsx
+++ b/score_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Utrip itineraries</t>
   </si>
@@ -37,11 +37,26 @@
   <si>
     <t>Beamsearch</t>
   </si>
+  <si>
+    <t>Beamsarch k values</t>
+  </si>
+  <si>
+    <t>No result</t>
+  </si>
+  <si>
+    <t>runtime (seconds)</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>Backtrack results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,16 +402,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="18.140625" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +428,20 @@
       <c r="L1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>115.205842969</v>
       </c>
@@ -422,8 +454,17 @@
       <c r="L2">
         <v>126.642203831</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <v>63</v>
+      </c>
+      <c r="U2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2">
+        <v>129.514129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-11195.367629599999</v>
       </c>
@@ -433,88 +474,157 @@
       <c r="L3">
         <v>125.37092808200001</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>64</v>
+      </c>
+      <c r="U3">
+        <v>160.3237</v>
+      </c>
+      <c r="V3" s="1">
+        <v>7.9849537037037034E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H4">
         <v>141.369745263</v>
       </c>
       <c r="L4">
         <v>119.192885659</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>100</v>
+      </c>
+      <c r="V4" s="1">
+        <v>3.1087962962962959E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H5">
         <v>-163.983244673</v>
       </c>
       <c r="L5">
         <v>111.186374632</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>90</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2.5138888888888892E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H6">
         <v>11.627562382400001</v>
       </c>
       <c r="L6">
         <v>143.34632753599999</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>80</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2.5520833333333331E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H7">
         <v>97.651382044000002</v>
       </c>
       <c r="L7">
         <v>81.950787211000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>70</v>
+      </c>
+      <c r="V7" s="1">
+        <v>2.6400462962962964E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H8">
         <v>24.252066082700001</v>
       </c>
       <c r="L8">
         <v>123.348333122</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>60</v>
+      </c>
+      <c r="V8" s="1">
+        <v>4.8356481481481491E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H9">
         <v>33.604224975400001</v>
       </c>
       <c r="L9">
         <v>141.39700936400001</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>50</v>
+      </c>
+      <c r="V9" s="1">
+        <v>3.4872685185185182E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H10">
         <v>32.753635095</v>
       </c>
       <c r="L10">
         <v>134.89700936400001</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>40</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2.5532407407407407E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H11">
         <v>8.5199763425800004E-2</v>
       </c>
       <c r="L11">
         <v>98.3174397051</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>30</v>
+      </c>
+      <c r="V11" s="1">
+        <v>2.5983796296296298E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H12">
         <v>124.22645946900001</v>
       </c>
       <c r="L12">
         <v>121.03048862952525</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>20</v>
+      </c>
+      <c r="V12" s="1">
+        <v>2.6273148148148152E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H13">
         <v>186.58644173100001</v>
       </c>
       <c r="L13">
         <v>118.32050007970507</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="V13" s="1">
+        <v>5.4212962962962966E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H14">
         <v>128.628108191</v>
       </c>
@@ -522,7 +632,7 @@
         <v>132.85807826320311</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H15">
         <v>18.349851364999999</v>
       </c>
@@ -530,7 +640,7 @@
         <v>122.40655328792768</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H16">
         <v>86.026980595400005</v>
       </c>
@@ -1216,6 +1326,21 @@
       </c>
       <c r="L101">
         <v>129.99360698219269</v>
+      </c>
+    </row>
+    <row r="109" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L109">
+        <v>158.72720000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L110">
+        <v>160.3237</v>
+      </c>
+    </row>
+    <row r="111" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L111">
+        <v>170.29347000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>